<commit_message>
convert svg text to vector
</commit_message>
<xml_diff>
--- a/data/Columnbia_equity.xlsx
+++ b/data/Columnbia_equity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mio/Documents/GitHub/ms1-project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB207AD-1391-AA4E-AA1A-562E4DCC616C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{409BA879-9F97-E14F-8294-07B9705C21C6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1260" windowWidth="29560" windowHeight="15540" activeTab="3" xr2:uid="{6C135D8D-6422-A449-8018-F89CA677DF0A}"/>
+    <workbookView xWindow="0" yWindow="1260" windowWidth="28800" windowHeight="15540" activeTab="1" xr2:uid="{6C135D8D-6422-A449-8018-F89CA677DF0A}"/>
   </bookViews>
   <sheets>
     <sheet name="% women in each rank" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2292,7 +2292,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EE6F78C-8743-414D-B74F-1C927A66602A}">
   <dimension ref="A1:AC28"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
@@ -3684,8 +3684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F87AFAD2-F9CB-A24A-AE0F-CD50D523E1FC}">
   <dimension ref="A1:T15"/>
   <sheetViews>
-    <sheetView zoomScale="75" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD15"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4419,7 +4419,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C54C599-C133-984D-A238-E2CAD5B217AC}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>

</xml_diff>